<commit_message>
Activiter créés et navigation entre aussi
</commit_message>
<xml_diff>
--- a/Projet_Android_MPE.xlsx
+++ b/Projet_Android_MPE.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\533\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\533\Desktop\OMEGALUL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="34">
   <si>
     <t>ID</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>En tant qu'utilisateur, je souhaite pouvoir finir la partie afin de pouvoir gagner la partie</t>
+  </si>
+  <si>
+    <t>Bouton pour commencer une nouvelle partie</t>
   </si>
 </sst>
 </file>
@@ -569,7 +572,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -636,7 +639,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="9" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>